<commit_message>
Curating transporters and cross-referencing genes with omics data
</commit_message>
<xml_diff>
--- a/model_building/transporters/Transporters (clean).xlsx
+++ b/model_building/transporters/Transporters (clean).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a30fe02b4181869d/SchoolWork/Stanford Grad/Projects/Covert Lab/Oceans/rpom-fba/model_building/transporters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="11_F25DC773A252ABDACC10489549185EAA5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C9CDFEA-4ECD-4C75-B8CF-6311794C9EAD}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="11_F25DC773A252ABDACC10489549185EAA5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DA11A5C-8109-4CB1-8E88-B6A2FABC0AF7}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-4290" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="480">
   <si>
     <t>Transporter ID</t>
   </si>
@@ -1318,14 +1318,161 @@
     <t>Transporter type</t>
   </si>
   <si>
-    <t>ATP + S[e] -&gt; ADP + Pi + S[c]</t>
+    <t>x ATP + S[e] -&gt; x ADP + x Pi + S[c]</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>x is difficult to determine, but in the absence of more information, assume 2 (see https://pmc.ncbi.nlm.nih.gov/articles/PMC3971661/)</t>
+  </si>
+  <si>
+    <t>See also interesting article about component ratios https://www.biorxiv.org/content/10.1101/2025.02.23.639702v1.full</t>
+  </si>
+  <si>
+    <t>x ION [e] + S[e] -&gt; x ION[c] + S[c]</t>
+  </si>
+  <si>
+    <t>https://www.cell.com/trends/biochemical-sciences/fulltext/S0968-0004(23)00295-5</t>
+  </si>
+  <si>
+    <t>Ion is (always?) Na+, x &gt;= 2. Used for acids</t>
+  </si>
+  <si>
+    <t>Betaine/Carnitine/Choline Transporter family. Can be driven by proton gradient, Na+ gradient, or substrate antiport... (https://tcdb.org/search/result.php?tc=2.A.15)</t>
+  </si>
+  <si>
+    <t>Tripartite tricarboxylate transporter family. See this one involved in citrate uptake? https://www.researchgate.net/publication/333157787_A_tripartite_tricarboxylate_transporter_MIM_c39170-MIM_c39210_of_Advenella_mimigardefordensis_DPN7T_is_involved_in_citrate_uptake</t>
+  </si>
+  <si>
+    <t>See downstream SPO1510, 1511 for possible permease and ATP-binding casette?</t>
+  </si>
+  <si>
+    <t>Note that E. coli uses a phosphotransferase system, and R. pom has the enzyme to degrade the phosphorylated version of this molecule… (https://biocyc.org/pathway?orgid=RUEGERIA_POMEROYI_DSS3&amp;id=GLUAMCAT-PWY)</t>
+  </si>
+  <si>
+    <t>Malate</t>
+  </si>
+  <si>
+    <t>Succinate</t>
+  </si>
+  <si>
+    <t>Fumarate</t>
+  </si>
+  <si>
+    <t>Xylose</t>
+  </si>
+  <si>
+    <t>Glucose</t>
+  </si>
+  <si>
+    <t>Cadaverine</t>
+  </si>
+  <si>
+    <t>Putrescine</t>
+  </si>
+  <si>
+    <t>Spermidine</t>
+  </si>
+  <si>
+    <t>In growth data?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>BioCyc ID</t>
+  </si>
+  <si>
+    <t>CPD-335</t>
+  </si>
+  <si>
+    <t>CPD0-1265</t>
+  </si>
+  <si>
+    <t>Grows?</t>
+  </si>
+  <si>
+    <t>Model grows?</t>
+  </si>
+  <si>
+    <t>CARNITINE</t>
+  </si>
+  <si>
+    <t>CIT</t>
+  </si>
+  <si>
+    <t>L-CYSTEATE</t>
+  </si>
+  <si>
+    <t>CPD-12692</t>
+  </si>
+  <si>
+    <t>SS-DIMETHYL-BETA-PROPIOTHETIN</t>
+  </si>
+  <si>
+    <t>ECTOINE</t>
+  </si>
+  <si>
+    <t>FUM</t>
+  </si>
+  <si>
+    <t>MAL</t>
+  </si>
+  <si>
+    <t>SUC</t>
+  </si>
+  <si>
+    <t>GLC</t>
+  </si>
+  <si>
+    <t>CPD-25028</t>
+  </si>
+  <si>
+    <t>GLYCEROL</t>
+  </si>
+  <si>
+    <t>GLYCEROL-3P</t>
+  </si>
+  <si>
+    <t>CPD-3745</t>
+  </si>
+  <si>
+    <t>N-ACETYL-D-GLUCOSAMINE</t>
+  </si>
+  <si>
+    <t>SPERMIDINE</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>CADAVERINE</t>
+  </si>
+  <si>
+    <t>PUTRESCINE</t>
+  </si>
+  <si>
+    <t>TAURINE</t>
+  </si>
+  <si>
+    <t>THYMIDINE</t>
+  </si>
+  <si>
+    <t>No - but trimethylamine, which is processed to TMAO, is</t>
+  </si>
+  <si>
+    <t>No (missing)</t>
+  </si>
+  <si>
+    <t>!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1341,13 +1488,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0F0F0F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1359,14 +1526,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1380,6 +1558,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1647,21 +1829,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.26953125" customWidth="1"/>
-    <col min="3" max="3" width="33.453125" customWidth="1"/>
-    <col min="4" max="4" width="43" customWidth="1"/>
-    <col min="5" max="5" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" customWidth="1"/>
+    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1681,10 +1863,10 @@
         <v>423</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -1700,8 +1882,11 @@
       <c r="F2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G2" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>194</v>
       </c>
@@ -1718,7 +1903,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>221</v>
       </c>
@@ -1735,7 +1920,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -1752,7 +1937,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1769,7 +1954,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>224</v>
       </c>
@@ -1786,7 +1971,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1803,7 +1988,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>229</v>
       </c>
@@ -1820,7 +2005,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -1837,7 +2022,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>199</v>
       </c>
@@ -1854,7 +2039,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -1871,7 +2056,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1888,7 +2073,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1905,7 +2090,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>175</v>
       </c>
@@ -1922,7 +2107,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -1938,8 +2123,11 @@
       <c r="F16" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -1956,7 +2144,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>238</v>
       </c>
@@ -1973,7 +2161,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1990,7 +2178,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -2007,7 +2195,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -2024,7 +2212,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2038,7 +2226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -2052,7 +2240,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -2069,7 +2257,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -2086,7 +2274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -2100,7 +2288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -2114,7 +2302,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2128,7 +2316,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -2145,7 +2333,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -2162,7 +2350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -2176,7 +2364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2190,7 +2378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -2204,7 +2392,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -2218,7 +2406,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -2232,7 +2420,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -2246,7 +2434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -2260,7 +2448,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -2274,7 +2462,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -2288,7 +2476,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -2302,7 +2490,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -2316,7 +2504,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -2330,7 +2518,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -2344,7 +2532,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>81</v>
       </c>
@@ -2358,7 +2546,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -2372,7 +2560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -2386,7 +2574,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>88</v>
       </c>
@@ -2400,7 +2588,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>95</v>
       </c>
@@ -2414,7 +2602,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -2428,7 +2616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>102</v>
       </c>
@@ -2442,7 +2630,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -2456,7 +2644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>107</v>
       </c>
@@ -2470,7 +2658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -2484,7 +2672,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -2498,7 +2686,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>113</v>
       </c>
@@ -2512,7 +2700,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>115</v>
       </c>
@@ -2526,7 +2714,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>117</v>
       </c>
@@ -2540,7 +2728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>122</v>
       </c>
@@ -2554,7 +2742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>124</v>
       </c>
@@ -2568,7 +2756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>129</v>
       </c>
@@ -2582,7 +2770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>131</v>
       </c>
@@ -2596,7 +2784,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>133</v>
       </c>
@@ -2610,7 +2798,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>135</v>
       </c>
@@ -2624,7 +2812,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>137</v>
       </c>
@@ -2638,7 +2826,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>139</v>
       </c>
@@ -2652,7 +2840,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>141</v>
       </c>
@@ -2666,7 +2854,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>143</v>
       </c>
@@ -2680,7 +2868,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>145</v>
       </c>
@@ -2694,7 +2882,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>147</v>
       </c>
@@ -2708,7 +2896,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>150</v>
       </c>
@@ -2722,7 +2910,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>152</v>
       </c>
@@ -2736,7 +2924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>154</v>
       </c>
@@ -2750,7 +2938,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>159</v>
       </c>
@@ -2764,7 +2952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>161</v>
       </c>
@@ -2778,7 +2966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>163</v>
       </c>
@@ -2792,7 +2980,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>165</v>
       </c>
@@ -2806,7 +2994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>167</v>
       </c>
@@ -2820,7 +3008,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>170</v>
       </c>
@@ -2834,7 +3022,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>172</v>
       </c>
@@ -2848,7 +3036,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>178</v>
       </c>
@@ -2862,7 +3050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>180</v>
       </c>
@@ -2876,7 +3064,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>182</v>
       </c>
@@ -2890,7 +3078,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>184</v>
       </c>
@@ -2904,7 +3092,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>186</v>
       </c>
@@ -2918,7 +3106,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>188</v>
       </c>
@@ -2932,7 +3120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>190</v>
       </c>
@@ -2946,7 +3134,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>192</v>
       </c>
@@ -2960,7 +3148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>197</v>
       </c>
@@ -2974,7 +3162,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>202</v>
       </c>
@@ -2988,7 +3176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>204</v>
       </c>
@@ -3002,7 +3190,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>206</v>
       </c>
@@ -3016,7 +3204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>208</v>
       </c>
@@ -3030,7 +3218,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>211</v>
       </c>
@@ -3044,7 +3232,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>214</v>
       </c>
@@ -3058,7 +3246,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>216</v>
       </c>
@@ -3072,7 +3260,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>218</v>
       </c>
@@ -3086,7 +3274,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>227</v>
       </c>
@@ -3100,7 +3288,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>232</v>
       </c>
@@ -3114,7 +3302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>234</v>
       </c>
@@ -3128,7 +3316,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>236</v>
       </c>
@@ -3142,7 +3330,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>241</v>
       </c>
@@ -3156,7 +3344,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>243</v>
       </c>
@@ -3170,7 +3358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>245</v>
       </c>
@@ -3184,7 +3372,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>247</v>
       </c>
@@ -3198,7 +3386,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>249</v>
       </c>
@@ -3212,7 +3400,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>251</v>
       </c>
@@ -3226,7 +3414,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>253</v>
       </c>
@@ -3240,7 +3428,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>255</v>
       </c>
@@ -3254,7 +3442,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>257</v>
       </c>
@@ -3268,7 +3456,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>259</v>
       </c>
@@ -3282,7 +3470,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>261</v>
       </c>
@@ -3296,7 +3484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>263</v>
       </c>
@@ -3310,7 +3498,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>265</v>
       </c>
@@ -3324,7 +3512,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>267</v>
       </c>
@@ -3338,7 +3526,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>269</v>
       </c>
@@ -3352,7 +3540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>271</v>
       </c>
@@ -3366,7 +3554,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>273</v>
       </c>
@@ -3380,7 +3568,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>275</v>
       </c>
@@ -3394,7 +3582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>277</v>
       </c>
@@ -3408,7 +3596,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>279</v>
       </c>
@@ -3422,7 +3610,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>281</v>
       </c>
@@ -3436,7 +3624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>283</v>
       </c>
@@ -3450,7 +3638,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>285</v>
       </c>
@@ -3464,7 +3652,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>287</v>
       </c>
@@ -3478,7 +3666,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>290</v>
       </c>
@@ -3492,7 +3680,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>292</v>
       </c>
@@ -3506,7 +3694,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>294</v>
       </c>
@@ -3531,132 +3719,581 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828A4D80-C8C6-4787-92CF-F703D94AFC6E}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>429</v>
       </c>
       <c r="B1" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="D2" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>434</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="D3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" s="3" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>289</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>451</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>121</v>
+      </c>
+      <c r="B25" t="s">
+        <v>450</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>196</v>
+      </c>
+      <c r="B26" t="s">
+        <v>450</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="D26" t="s">
+        <v>450</v>
+      </c>
+      <c r="E26" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>223</v>
+      </c>
+      <c r="B27" t="s">
+        <v>450</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>450</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="s">
+        <v>450</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="D29" t="s">
+        <v>450</v>
+      </c>
+      <c r="E29" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>226</v>
+      </c>
+      <c r="B30" t="s">
+        <v>450</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="D30" t="s">
+        <v>450</v>
+      </c>
+      <c r="E30" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>450</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="D31" t="s">
+        <v>450</v>
+      </c>
+      <c r="E31" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>231</v>
+      </c>
+      <c r="B32" t="s">
+        <v>450</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" t="s">
+        <v>450</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="D33" t="s">
+        <v>450</v>
+      </c>
+      <c r="E33" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>443</v>
+      </c>
+      <c r="B34" t="s">
+        <v>450</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="D34" t="s">
+        <v>450</v>
+      </c>
+      <c r="E34" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>441</v>
+      </c>
+      <c r="B35" t="s">
+        <v>450</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="D35" t="s">
+        <v>450</v>
+      </c>
+      <c r="E35" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>442</v>
+      </c>
+      <c r="B36" t="s">
+        <v>450</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="D36" t="s">
+        <v>450</v>
+      </c>
+      <c r="E36" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>445</v>
+      </c>
+      <c r="B37" t="s">
+        <v>450</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="D37" t="s">
+        <v>450</v>
+      </c>
+      <c r="E37" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>444</v>
+      </c>
+      <c r="B38" t="s">
+        <v>450</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="D38" t="s">
+        <v>450</v>
+      </c>
+      <c r="E38" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" t="s">
+        <v>450</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D39" t="s">
+        <v>450</v>
+      </c>
+      <c r="E39" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" t="s">
+        <v>450</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41" t="s">
+        <v>450</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="D41" t="s">
+        <v>450</v>
+      </c>
+      <c r="E41" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>158</v>
+      </c>
+      <c r="B42" t="s">
+        <v>450</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="D42" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>448</v>
+      </c>
+      <c r="B44" t="s">
+        <v>450</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="D44" t="s">
+        <v>450</v>
+      </c>
+      <c r="E44" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>446</v>
+      </c>
+      <c r="B45" t="s">
+        <v>450</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>450</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>447</v>
+      </c>
+      <c r="B46" t="s">
+        <v>450</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="D46" t="s">
+        <v>450</v>
+      </c>
+      <c r="E46" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" t="s">
+        <v>450</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="D47" t="s">
+        <v>450</v>
+      </c>
+      <c r="E47" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" t="s">
+        <v>450</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="D48" t="s">
+        <v>450</v>
+      </c>
+      <c r="E48" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>128</v>
+      </c>
+      <c r="B49" t="s">
+        <v>477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work on curating catabolic pathways
</commit_message>
<xml_diff>
--- a/model_building/transporters/Transporters (clean).xlsx
+++ b/model_building/transporters/Transporters (clean).xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="229" documentId="11_F25DC773A252ABDACC10489549185EAA5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DA11A5C-8109-4CB1-8E88-B6A2FABC0AF7}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-4290" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1829,8 +1829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3721,8 +3721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828A4D80-C8C6-4787-92CF-F703D94AFC6E}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25:E25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
work on catabolic pathway curation, keeping genes necessary for alternative substrates
</commit_message>
<xml_diff>
--- a/model_building/transporters/Transporters (clean).xlsx
+++ b/model_building/transporters/Transporters (clean).xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="229" documentId="11_F25DC773A252ABDACC10489549185EAA5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DA11A5C-8109-4CB1-8E88-B6A2FABC0AF7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-4290" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1829,8 +1829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3721,8 +3721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828A4D80-C8C6-4787-92CF-F703D94AFC6E}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixing valine, glutamate growth (had to re-make index, a lot of random files added
</commit_message>
<xml_diff>
--- a/model_building/transporters/Transporters (clean).xlsx
+++ b/model_building/transporters/Transporters (clean).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a30fe02b4181869d/SchoolWork/Stanford Grad/Projects/Covert Lab/Oceans/rpom-fba/model_building/transporters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="229" documentId="11_F25DC773A252ABDACC10489549185EAA5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DA11A5C-8109-4CB1-8E88-B6A2FABC0AF7}"/>
+  <xr:revisionPtr revIDLastSave="232" documentId="11_F25DC773A252ABDACC10489549185EAA5BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9BDE92A-504E-4C09-BDF4-AE813273EB70}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-4290" windowWidth="16440" windowHeight="28320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="481">
   <si>
     <t>Transporter ID</t>
   </si>
@@ -1466,6 +1466,9 @@
   </si>
   <si>
     <t>!!</t>
+  </si>
+  <si>
+    <t>Adding this</t>
   </si>
 </sst>
 </file>
@@ -1503,7 +1506,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1513,6 +1516,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1530,7 +1539,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1542,6 +1551,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1829,21 +1839,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" customWidth="1"/>
-    <col min="6" max="6" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.26953125" customWidth="1"/>
+    <col min="3" max="3" width="33.453125" customWidth="1"/>
+    <col min="4" max="4" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" customWidth="1"/>
+    <col min="6" max="6" width="34.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1866,7 +1876,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>119</v>
       </c>
@@ -1886,7 +1896,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>194</v>
       </c>
@@ -1903,7 +1913,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>221</v>
       </c>
@@ -1920,7 +1930,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>91</v>
       </c>
@@ -1937,7 +1947,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1954,7 +1964,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>224</v>
       </c>
@@ -1971,7 +1981,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1988,7 +1998,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>229</v>
       </c>
@@ -2005,7 +2015,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -2022,7 +2032,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>199</v>
       </c>
@@ -2039,7 +2049,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -2056,7 +2066,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2073,7 +2083,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -2090,7 +2100,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>175</v>
       </c>
@@ -2107,7 +2117,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>156</v>
       </c>
@@ -2127,7 +2137,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -2144,7 +2154,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>238</v>
       </c>
@@ -2161,7 +2171,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -2178,7 +2188,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -2195,7 +2205,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>126</v>
       </c>
@@ -2212,7 +2222,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -2226,7 +2236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -2240,7 +2250,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -2257,7 +2267,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -2274,7 +2284,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -2288,7 +2298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -2302,7 +2312,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -2316,7 +2326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -2333,24 +2343,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="7" t="s">
         <v>427</v>
       </c>
-      <c r="E30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E30" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>34</v>
       </c>
@@ -2364,7 +2377,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -2378,7 +2391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>51</v>
       </c>
@@ -2392,7 +2405,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -2406,7 +2419,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -2420,7 +2433,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -2434,7 +2447,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>60</v>
       </c>
@@ -2448,7 +2461,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>62</v>
       </c>
@@ -2462,7 +2475,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>65</v>
       </c>
@@ -2476,7 +2489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -2490,7 +2503,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -2504,7 +2517,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -2518,7 +2531,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -2532,7 +2545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>81</v>
       </c>
@@ -2546,7 +2559,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>84</v>
       </c>
@@ -2560,7 +2573,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -2574,7 +2587,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>88</v>
       </c>
@@ -2588,7 +2601,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>95</v>
       </c>
@@ -2602,7 +2615,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>97</v>
       </c>
@@ -2616,7 +2629,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>102</v>
       </c>
@@ -2630,7 +2643,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>105</v>
       </c>
@@ -2644,7 +2657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>107</v>
       </c>
@@ -2658,7 +2671,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -2672,7 +2685,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>111</v>
       </c>
@@ -2686,7 +2699,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>113</v>
       </c>
@@ -2700,7 +2713,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>115</v>
       </c>
@@ -2714,7 +2727,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>117</v>
       </c>
@@ -2728,7 +2741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>122</v>
       </c>
@@ -2742,7 +2755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>124</v>
       </c>
@@ -2756,7 +2769,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>129</v>
       </c>
@@ -2770,7 +2783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>131</v>
       </c>
@@ -2784,7 +2797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>133</v>
       </c>
@@ -2798,7 +2811,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>135</v>
       </c>
@@ -2812,7 +2825,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>137</v>
       </c>
@@ -2826,7 +2839,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>139</v>
       </c>
@@ -2840,7 +2853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>141</v>
       </c>
@@ -2854,7 +2867,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>143</v>
       </c>
@@ -2868,7 +2881,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>145</v>
       </c>
@@ -2882,7 +2895,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>147</v>
       </c>
@@ -2896,7 +2909,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>150</v>
       </c>
@@ -2910,7 +2923,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>152</v>
       </c>
@@ -2924,7 +2937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>154</v>
       </c>
@@ -2938,7 +2951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>159</v>
       </c>
@@ -2952,7 +2965,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>161</v>
       </c>
@@ -2966,7 +2979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>163</v>
       </c>
@@ -2980,7 +2993,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>165</v>
       </c>
@@ -2994,7 +3007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>167</v>
       </c>
@@ -3008,7 +3021,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>170</v>
       </c>
@@ -3022,7 +3035,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>172</v>
       </c>
@@ -3036,7 +3049,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>178</v>
       </c>
@@ -3050,7 +3063,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>180</v>
       </c>
@@ -3064,7 +3077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>182</v>
       </c>
@@ -3078,7 +3091,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>184</v>
       </c>
@@ -3092,7 +3105,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>186</v>
       </c>
@@ -3106,7 +3119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>188</v>
       </c>
@@ -3120,7 +3133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>190</v>
       </c>
@@ -3134,7 +3147,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>192</v>
       </c>
@@ -3148,7 +3161,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>197</v>
       </c>
@@ -3162,7 +3175,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>202</v>
       </c>
@@ -3176,7 +3189,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>204</v>
       </c>
@@ -3190,7 +3203,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>206</v>
       </c>
@@ -3204,7 +3217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>208</v>
       </c>
@@ -3218,7 +3231,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>211</v>
       </c>
@@ -3232,7 +3245,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>214</v>
       </c>
@@ -3246,7 +3259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>216</v>
       </c>
@@ -3260,7 +3273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>218</v>
       </c>
@@ -3274,7 +3287,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>227</v>
       </c>
@@ -3288,7 +3301,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>232</v>
       </c>
@@ -3302,7 +3315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>234</v>
       </c>
@@ -3316,7 +3329,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>236</v>
       </c>
@@ -3330,7 +3343,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>241</v>
       </c>
@@ -3344,7 +3357,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>243</v>
       </c>
@@ -3358,7 +3371,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>245</v>
       </c>
@@ -3372,7 +3385,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>247</v>
       </c>
@@ -3386,7 +3399,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>249</v>
       </c>
@@ -3400,7 +3413,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>251</v>
       </c>
@@ -3414,7 +3427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>253</v>
       </c>
@@ -3428,7 +3441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>255</v>
       </c>
@@ -3442,7 +3455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>257</v>
       </c>
@@ -3456,7 +3469,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>259</v>
       </c>
@@ -3470,7 +3483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>261</v>
       </c>
@@ -3484,7 +3497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>263</v>
       </c>
@@ -3498,7 +3511,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>265</v>
       </c>
@@ -3512,7 +3525,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>267</v>
       </c>
@@ -3526,7 +3539,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>269</v>
       </c>
@@ -3540,7 +3553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>271</v>
       </c>
@@ -3554,7 +3567,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>273</v>
       </c>
@@ -3568,7 +3581,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>275</v>
       </c>
@@ -3582,7 +3595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>277</v>
       </c>
@@ -3596,7 +3609,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>279</v>
       </c>
@@ -3610,7 +3623,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>281</v>
       </c>
@@ -3624,7 +3637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>283</v>
       </c>
@@ -3638,7 +3651,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>285</v>
       </c>
@@ -3652,7 +3665,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>287</v>
       </c>
@@ -3666,7 +3679,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>290</v>
       </c>
@@ -3680,7 +3693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>292</v>
       </c>
@@ -3694,7 +3707,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>294</v>
       </c>
@@ -3721,20 +3734,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{828A4D80-C8C6-4787-92CF-F703D94AFC6E}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25:E25"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="3" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>429</v>
       </c>
@@ -3745,7 +3758,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -3759,7 +3772,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -3773,7 +3786,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -3782,7 +3795,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="145" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -3790,92 +3803,92 @@
         <v>438</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>449</v>
       </c>
@@ -3889,7 +3902,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>121</v>
       </c>
@@ -3906,7 +3919,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>196</v>
       </c>
@@ -3923,7 +3936,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>223</v>
       </c>
@@ -3940,7 +3953,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>94</v>
       </c>
@@ -3957,7 +3970,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -3974,7 +3987,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>226</v>
       </c>
@@ -3991,7 +4004,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -4008,7 +4021,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>231</v>
       </c>
@@ -4025,7 +4038,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -4042,7 +4055,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>443</v>
       </c>
@@ -4059,7 +4072,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>441</v>
       </c>
@@ -4076,7 +4089,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>442</v>
       </c>
@@ -4093,7 +4106,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>445</v>
       </c>
@@ -4110,7 +4123,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>444</v>
       </c>
@@ -4127,7 +4140,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>42</v>
       </c>
@@ -4144,7 +4157,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>24</v>
       </c>
@@ -4164,7 +4177,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>177</v>
       </c>
@@ -4181,7 +4194,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>158</v>
       </c>
@@ -4195,7 +4208,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -4203,7 +4216,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>448</v>
       </c>
@@ -4220,7 +4233,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>446</v>
       </c>
@@ -4237,7 +4250,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>447</v>
       </c>
@@ -4254,7 +4267,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -4271,7 +4284,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>27</v>
       </c>
@@ -4288,7 +4301,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>128</v>
       </c>

</xml_diff>